<commit_message>
change excel url and fix assign tranportation order
</commit_message>
<xml_diff>
--- a/NhapHangV2.API/Template/AdminSendUserWalletReportTemplate.xlsx
+++ b/NhapHangV2.API/Template/AdminSendUserWalletReportTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mona\NhapHangCore\NhapHangV2.API\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mona\nhaphangv2.monamedia.net\NhapHangV2.API\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF0E354-7002-4069-82F8-09EAF26E134F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A6B081-0914-4247-9894-D48F822A29FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1DEE34EF-099D-413C-A598-4D82A4FCF97F}"/>
   </bookViews>
@@ -20,16 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -84,7 +74,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -128,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -136,10 +126,16 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -459,14 +455,15 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.5546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.88671875" style="1" customWidth="1"/>
-    <col min="3" max="4" width="28.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="27.21875" style="1" customWidth="1"/>
     <col min="6" max="6" width="25.109375" style="4" customWidth="1"/>
     <col min="7" max="7" width="26.21875" style="1" customWidth="1"/>
@@ -480,7 +477,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -503,7 +500,7 @@
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="1" t="s">

</xml_diff>